<commit_message>
Apresentação final - update
</commit_message>
<xml_diff>
--- a/6OrganiçaoGrupo(Importante)/Tarefas_app.xlsx
+++ b/6OrganiçaoGrupo(Importante)/Tarefas_app.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="209" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="222" uniqueCount="83">
   <si>
     <t>Tarefa</t>
   </si>
@@ -66,9 +66,6 @@
     <t>Feito</t>
   </si>
   <si>
-    <t>A fazer...</t>
-  </si>
-  <si>
     <t>Guardar / extrair os dados (texto, imagens, som) da Base de dados (SQlight), no android</t>
   </si>
   <si>
@@ -231,9 +228,6 @@
     <t>Na execução sequencial do teste este verifica automaticamente qual o tipo e escolhe o layout adequado</t>
   </si>
   <si>
-    <t>Suspenso</t>
-  </si>
-  <si>
     <t>Testes texto/português</t>
   </si>
   <si>
@@ -262,6 +256,15 @@
   </si>
   <si>
     <t>Sincronizar as alterações Tablet/servidor/tablet</t>
+  </si>
+  <si>
+    <t>Suspenso / reposto</t>
+  </si>
+  <si>
+    <t>Sincronização manual</t>
+  </si>
+  <si>
+    <t>t</t>
   </si>
 </sst>
 </file>
@@ -285,7 +288,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="11">
+  <fills count="10">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -330,12 +333,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="3" tint="0.59999389629810485"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="6" tint="-0.249977111117893"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -736,7 +733,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="133">
+  <cellXfs count="114">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
@@ -755,16 +752,13 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="6" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -779,30 +773,18 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="29" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="9" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="10" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="15" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -819,6 +801,26 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -831,15 +833,6 @@
     <xf numFmtId="0" fontId="1" fillId="4" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -867,6 +860,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -883,15 +885,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
@@ -903,22 +896,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="9" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -945,31 +929,13 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="9" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -981,6 +947,15 @@
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -990,24 +965,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -1015,15 +972,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1330,15 +1278,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:H73"/>
+  <dimension ref="A1:I74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A27" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H56" sqref="H56"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="B10" sqref="B10:D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.140625" style="17" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="3.140625" style="16" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="31.42578125" customWidth="1"/>
     <col min="3" max="3" width="35.42578125" customWidth="1"/>
     <col min="4" max="4" width="46" customWidth="1"/>
@@ -1349,22 +1297,22 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="101" t="s">
+      <c r="B2" s="94" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="102"/>
-      <c r="D2" s="102"/>
+      <c r="C2" s="95"/>
+      <c r="D2" s="95"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="F2" s="4" t="s">
         <v>13</v>
       </c>
-      <c r="G2" s="22" t="s">
+      <c r="G2" s="20" t="s">
+        <v>59</v>
+      </c>
+      <c r="H2" s="35" t="s">
         <v>60</v>
-      </c>
-      <c r="H2" s="38" t="s">
-        <v>61</v>
       </c>
     </row>
     <row r="3" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -1374,7 +1322,7 @@
       <c r="E3" s="5" t="s">
         <v>2</v>
       </c>
-      <c r="H3" s="39"/>
+      <c r="H3" s="36"/>
     </row>
     <row r="4" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B4" s="2"/>
@@ -1383,7 +1331,7 @@
       <c r="E4" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="H4" s="39"/>
+      <c r="H4" s="36"/>
     </row>
     <row r="5" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B5" s="2"/>
@@ -1392,7 +1340,7 @@
       <c r="E5" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="H5" s="39"/>
+      <c r="H5" s="36"/>
     </row>
     <row r="6" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B6" s="2"/>
@@ -1401,7 +1349,7 @@
       <c r="E6" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="H6" s="39"/>
+      <c r="H6" s="36"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="2"/>
@@ -1410,7 +1358,7 @@
       <c r="E7" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="H7" s="39"/>
+      <c r="H7" s="36"/>
     </row>
     <row r="8" spans="1:8" ht="15.75" hidden="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B8" s="2"/>
@@ -1419,1255 +1367,1300 @@
       <c r="E8" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="H8" s="39"/>
+      <c r="H8" s="36"/>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="18">
+      <c r="A9" s="17">
         <v>1</v>
       </c>
-      <c r="B9" s="68" t="s">
+      <c r="B9" s="60" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="69"/>
-      <c r="D9" s="70"/>
+      <c r="C9" s="61"/>
+      <c r="D9" s="62"/>
       <c r="E9" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F9" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="G9" s="35" t="s">
-        <v>21</v>
-      </c>
-      <c r="H9" s="32"/>
+      <c r="F9" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="G9" s="32" t="s">
+        <v>20</v>
+      </c>
+      <c r="H9" s="29"/>
     </row>
     <row r="10" spans="1:8" ht="57" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A10" s="18">
+      <c r="A10" s="17">
         <f>A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="103" t="s">
+      <c r="B10" s="96" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="104"/>
-      <c r="D10" s="105"/>
-      <c r="E10" s="66" t="s">
-        <v>64</v>
-      </c>
-      <c r="F10" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G10" s="29" t="s">
+      <c r="C10" s="97"/>
+      <c r="D10" s="98"/>
+      <c r="E10" s="65" t="s">
+        <v>63</v>
+      </c>
+      <c r="F10" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G10" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H10" s="63" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="64" t="s">
-        <v>24</v>
-      </c>
     </row>
     <row r="11" spans="1:8" ht="37.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="18">
-        <f t="shared" ref="A11:A73" si="0">A10+1</f>
+      <c r="A11" s="17">
+        <f t="shared" ref="A11:A74" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="68" t="s">
+      <c r="B11" s="60" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="69"/>
-      <c r="D11" s="70"/>
-      <c r="E11" s="67"/>
-      <c r="F11" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G11" s="29" t="s">
-        <v>23</v>
-      </c>
-      <c r="H11" s="65"/>
+      <c r="C11" s="61"/>
+      <c r="D11" s="62"/>
+      <c r="E11" s="66"/>
+      <c r="F11" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G11" s="26" t="s">
+        <v>22</v>
+      </c>
+      <c r="H11" s="64"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="18">
+      <c r="A12" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="68" t="s">
-        <v>17</v>
-      </c>
-      <c r="C12" s="69"/>
-      <c r="D12" s="70"/>
+      <c r="B12" s="60" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" s="61"/>
+      <c r="D12" s="62"/>
       <c r="E12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="F12" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G12" s="29" t="s">
-        <v>21</v>
+        <v>26</v>
+      </c>
+      <c r="F12" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G12" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="H12" s="10"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="18">
+      <c r="A13" s="17">
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="68" t="s">
-        <v>29</v>
-      </c>
-      <c r="C13" s="69"/>
-      <c r="D13" s="70"/>
+      <c r="B13" s="60" t="s">
+        <v>28</v>
+      </c>
+      <c r="C13" s="61"/>
+      <c r="D13" s="62"/>
       <c r="E13" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F13" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G13" s="29" t="s">
-        <v>21</v>
+      <c r="F13" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G13" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="H13" s="10"/>
     </row>
-    <row r="14" spans="1:8" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="18">
+    <row r="14" spans="1:8" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A14" s="17">
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="115" t="s">
-        <v>39</v>
-      </c>
-      <c r="C14" s="116"/>
-      <c r="D14" s="117"/>
+      <c r="B14" s="102" t="s">
+        <v>38</v>
+      </c>
+      <c r="C14" s="103"/>
+      <c r="D14" s="104"/>
       <c r="E14" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F14" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G14" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H14" s="33"/>
-    </row>
-    <row r="15" spans="1:8" s="17" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="18">
+      <c r="F14" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G14" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H14" s="30"/>
+    </row>
+    <row r="15" spans="1:8" s="16" customFormat="1" ht="29.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A15" s="17">
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="109" t="s">
-        <v>38</v>
-      </c>
-      <c r="C15" s="110"/>
-      <c r="D15" s="111"/>
-      <c r="E15" s="16" t="s">
+      <c r="B15" s="102" t="s">
+        <v>37</v>
+      </c>
+      <c r="C15" s="103"/>
+      <c r="D15" s="104"/>
+      <c r="E15" s="14" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G15" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="H15" s="33"/>
+      <c r="F15" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G15" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H15" s="30"/>
     </row>
     <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" s="18">
+      <c r="A16" s="17">
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B16" s="68" t="s">
-        <v>30</v>
-      </c>
-      <c r="C16" s="69"/>
-      <c r="D16" s="70"/>
+      <c r="B16" s="60" t="s">
+        <v>29</v>
+      </c>
+      <c r="C16" s="61"/>
+      <c r="D16" s="62"/>
       <c r="E16" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F16" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G16" s="29" t="s">
-        <v>21</v>
+      <c r="F16" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G16" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="H16" s="10"/>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" s="18">
+      <c r="A17" s="17">
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B17" s="68" t="s">
+      <c r="B17" s="60" t="s">
+        <v>30</v>
+      </c>
+      <c r="C17" s="61"/>
+      <c r="D17" s="62"/>
+      <c r="E17" s="14" t="s">
+        <v>2</v>
+      </c>
+      <c r="F17" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G17" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H17" s="10"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A18" s="17">
+        <f t="shared" si="0"/>
+        <v>10</v>
+      </c>
+      <c r="B18" s="60" t="s">
         <v>31</v>
       </c>
-      <c r="C17" s="69"/>
-      <c r="D17" s="70"/>
-      <c r="E17" s="14" t="s">
-        <v>5</v>
-      </c>
-      <c r="F17" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G17" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H17" s="10"/>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" s="18">
-        <f t="shared" si="0"/>
-        <v>10</v>
-      </c>
-      <c r="B18" s="92" t="s">
-        <v>32</v>
-      </c>
-      <c r="C18" s="93"/>
-      <c r="D18" s="94"/>
-      <c r="E18" s="16" t="s">
-        <v>7</v>
-      </c>
-      <c r="F18" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G18" s="37" t="s">
-        <v>21</v>
+      <c r="C18" s="61"/>
+      <c r="D18" s="62"/>
+      <c r="E18" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F18" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G18" s="44" t="s">
+        <v>20</v>
       </c>
       <c r="H18" s="10"/>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A19" s="18">
+      <c r="A19" s="17">
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="112" t="s">
-        <v>40</v>
-      </c>
-      <c r="C19" s="113"/>
-      <c r="D19" s="114"/>
-      <c r="E19" s="19" t="s">
+      <c r="B19" s="105" t="s">
+        <v>39</v>
+      </c>
+      <c r="C19" s="106"/>
+      <c r="D19" s="107"/>
+      <c r="E19" s="18" t="s">
         <v>2</v>
       </c>
-      <c r="F19" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G19" s="29" t="s">
-        <v>21</v>
+      <c r="F19" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G19" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="H19" s="10"/>
     </row>
     <row r="20" spans="1:8" ht="27.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="18">
+      <c r="A20" s="17">
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="68" t="s">
+      <c r="B20" s="60" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="69"/>
-      <c r="D20" s="70"/>
+      <c r="C20" s="61"/>
+      <c r="D20" s="62"/>
       <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F20" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G20" s="29" t="s">
-        <v>23</v>
+      <c r="F20" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G20" s="26" t="s">
+        <v>22</v>
       </c>
       <c r="H20" s="10"/>
     </row>
     <row r="21" spans="1:8" ht="27" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="18">
+      <c r="A21" s="17">
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="74" t="s">
-        <v>33</v>
-      </c>
-      <c r="C21" s="75"/>
-      <c r="D21" s="76"/>
+      <c r="B21" s="70" t="s">
+        <v>32</v>
+      </c>
+      <c r="C21" s="71"/>
+      <c r="D21" s="72"/>
       <c r="E21" s="7"/>
-      <c r="F21" s="27"/>
-      <c r="G21" s="29"/>
+      <c r="F21" s="24"/>
+      <c r="G21" s="26"/>
       <c r="H21" s="10"/>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A22" s="18">
+      <c r="A22" s="17">
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="68" t="s">
-        <v>18</v>
-      </c>
-      <c r="C22" s="69"/>
-      <c r="D22" s="70"/>
+      <c r="B22" s="60" t="s">
+        <v>17</v>
+      </c>
+      <c r="C22" s="61"/>
+      <c r="D22" s="62"/>
       <c r="E22" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F22" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G22" s="37" t="s">
-        <v>23</v>
-      </c>
-      <c r="H22" s="34" t="s">
-        <v>41</v>
+      <c r="F22" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G22" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="H22" s="31" t="s">
+        <v>40</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A23" s="18">
-        <f t="shared" si="0"/>
-        <v>15</v>
-      </c>
-      <c r="B23" s="68" t="s">
-        <v>19</v>
-      </c>
-      <c r="C23" s="69"/>
-      <c r="D23" s="70"/>
+      <c r="A23" s="17">
+        <f t="shared" si="0"/>
+        <v>15</v>
+      </c>
+      <c r="B23" s="60" t="s">
+        <v>18</v>
+      </c>
+      <c r="C23" s="61"/>
+      <c r="D23" s="62"/>
       <c r="E23" s="12" t="s">
+        <v>26</v>
+      </c>
+      <c r="F23" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G23" s="26" t="s">
+        <v>20</v>
+      </c>
+      <c r="H23" s="10"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A24" s="17">
+        <f t="shared" si="0"/>
+        <v>16</v>
+      </c>
+      <c r="B24" s="60" t="s">
+        <v>10</v>
+      </c>
+      <c r="C24" s="61"/>
+      <c r="D24" s="62"/>
+      <c r="E24" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="F24" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G24" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F23" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G23" s="29" t="s">
-        <v>21</v>
-      </c>
-      <c r="H23" s="10"/>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A24" s="18">
-        <f t="shared" si="0"/>
-        <v>16</v>
-      </c>
-      <c r="B24" s="86" t="s">
-        <v>10</v>
-      </c>
-      <c r="C24" s="87"/>
-      <c r="D24" s="88"/>
-      <c r="E24" s="56"/>
-      <c r="F24" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G24" s="54" t="s">
-        <v>28</v>
-      </c>
       <c r="H24" s="10"/>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A25" s="18">
+      <c r="A25" s="17">
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="68" t="s">
-        <v>58</v>
-      </c>
-      <c r="C25" s="69"/>
-      <c r="D25" s="70"/>
+      <c r="B25" s="60" t="s">
+        <v>57</v>
+      </c>
+      <c r="C25" s="61"/>
+      <c r="D25" s="62"/>
       <c r="E25" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F25" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G25" s="52" t="s">
-        <v>28</v>
+      <c r="F25" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G25" s="44" t="s">
+        <v>27</v>
       </c>
       <c r="H25" s="10"/>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A26" s="18">
+      <c r="A26" s="17">
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="95" t="s">
+      <c r="B26" s="88" t="s">
+        <v>64</v>
+      </c>
+      <c r="C26" s="89"/>
+      <c r="D26" s="90"/>
+      <c r="E26" s="37" t="s">
+        <v>26</v>
+      </c>
+      <c r="F26" s="38" t="s">
+        <v>15</v>
+      </c>
+      <c r="G26" s="39" t="s">
+        <v>27</v>
+      </c>
+      <c r="H26" s="40"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A27" s="17">
+        <f t="shared" si="0"/>
+        <v>19</v>
+      </c>
+      <c r="B27" s="99" t="s">
         <v>65</v>
       </c>
-      <c r="C26" s="96"/>
-      <c r="D26" s="97"/>
-      <c r="E26" s="44" t="s">
+      <c r="C27" s="100"/>
+      <c r="D27" s="101"/>
+      <c r="E27" s="41" t="s">
+        <v>26</v>
+      </c>
+      <c r="F27" s="39" t="s">
+        <v>15</v>
+      </c>
+      <c r="G27" s="39" t="s">
         <v>27</v>
       </c>
-      <c r="F26" s="45" t="s">
-        <v>15</v>
-      </c>
-      <c r="G26" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H26" s="47"/>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" s="18">
-        <f t="shared" si="0"/>
-        <v>19</v>
-      </c>
-      <c r="B27" s="106" t="s">
+      <c r="H27" s="40" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A28" s="17">
+        <f t="shared" si="0"/>
+        <v>20</v>
+      </c>
+      <c r="B28" s="51" t="s">
         <v>66</v>
       </c>
-      <c r="C27" s="107"/>
-      <c r="D27" s="108"/>
-      <c r="E27" s="48" t="s">
+      <c r="C28" s="52"/>
+      <c r="D28" s="53"/>
+      <c r="E28" s="49" t="s">
+        <v>26</v>
+      </c>
+      <c r="F28" s="50" t="s">
+        <v>15</v>
+      </c>
+      <c r="G28" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="H28" s="42"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A29" s="17">
+        <f t="shared" si="0"/>
+        <v>21</v>
+      </c>
+      <c r="B29" s="55" t="s">
+        <v>46</v>
+      </c>
+      <c r="C29" s="56"/>
+      <c r="D29" s="57"/>
+      <c r="E29" s="47"/>
+      <c r="F29" s="25" t="s">
+        <v>14</v>
+      </c>
+      <c r="G29" s="46" t="s">
         <v>27</v>
       </c>
-      <c r="F27" s="46" t="s">
-        <v>15</v>
-      </c>
-      <c r="G27" s="46" t="s">
-        <v>28</v>
-      </c>
-      <c r="H27" s="47" t="s">
-        <v>68</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A28" s="18">
-        <f t="shared" si="0"/>
-        <v>20</v>
-      </c>
-      <c r="B28" s="60" t="s">
-        <v>67</v>
-      </c>
-      <c r="C28" s="61"/>
-      <c r="D28" s="62"/>
-      <c r="E28" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="F28" s="59" t="s">
-        <v>15</v>
-      </c>
-      <c r="G28" s="59" t="s">
+      <c r="H29" s="10"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A30" s="17">
+        <f t="shared" si="0"/>
+        <v>22</v>
+      </c>
+      <c r="B30" s="79"/>
+      <c r="C30" s="80"/>
+      <c r="D30" s="81"/>
+      <c r="E30" s="7"/>
+      <c r="F30" s="24"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="10"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A31" s="17">
+        <f t="shared" si="0"/>
+        <v>23</v>
+      </c>
+      <c r="B31" s="70" t="s">
         <v>45</v>
       </c>
-      <c r="H28" s="49"/>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" s="18">
-        <f t="shared" si="0"/>
-        <v>21</v>
-      </c>
-      <c r="B29" s="41" t="s">
-        <v>47</v>
-      </c>
-      <c r="C29" s="42"/>
-      <c r="D29" s="43"/>
-      <c r="E29" s="21"/>
-      <c r="F29" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G29" s="54" t="s">
-        <v>28</v>
-      </c>
-      <c r="H29" s="10"/>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A30" s="18">
-        <f t="shared" si="0"/>
-        <v>22</v>
-      </c>
-      <c r="B30" s="80"/>
-      <c r="C30" s="81"/>
-      <c r="D30" s="82"/>
-      <c r="E30" s="7"/>
-      <c r="F30" s="27"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="10"/>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" s="18">
-        <f t="shared" si="0"/>
-        <v>23</v>
-      </c>
-      <c r="B31" s="74" t="s">
-        <v>46</v>
-      </c>
-      <c r="C31" s="75"/>
-      <c r="D31" s="76"/>
+      <c r="C31" s="71"/>
+      <c r="D31" s="72"/>
       <c r="E31" s="7"/>
-      <c r="F31" s="27"/>
-      <c r="G31" s="29"/>
+      <c r="F31" s="24"/>
+      <c r="G31" s="26"/>
       <c r="H31" s="10"/>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A32" s="18">
+      <c r="A32" s="17">
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B32" s="98" t="s">
-        <v>54</v>
-      </c>
-      <c r="C32" s="99"/>
-      <c r="D32" s="100"/>
+      <c r="B32" s="91" t="s">
+        <v>53</v>
+      </c>
+      <c r="C32" s="92"/>
+      <c r="D32" s="93"/>
       <c r="E32" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F32" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G32" s="52" t="s">
-        <v>28</v>
+      <c r="F32" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G32" s="44" t="s">
+        <v>27</v>
       </c>
       <c r="H32" s="10"/>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A33" s="18">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A33" s="17">
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B33" s="98" t="s">
-        <v>55</v>
-      </c>
-      <c r="C33" s="99"/>
-      <c r="D33" s="100"/>
+      <c r="B33" s="91" t="s">
+        <v>54</v>
+      </c>
+      <c r="C33" s="92"/>
+      <c r="D33" s="93"/>
       <c r="E33" s="14" t="s">
         <v>2</v>
       </c>
-      <c r="F33" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G33" s="52" t="s">
+      <c r="F33" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G33" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H33" s="10"/>
+    </row>
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A34" s="17">
+        <f t="shared" si="0"/>
+        <v>26</v>
+      </c>
+      <c r="B34" s="91" t="s">
+        <v>48</v>
+      </c>
+      <c r="C34" s="92"/>
+      <c r="D34" s="93"/>
+      <c r="E34" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F34" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G34" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H34" s="10"/>
+      <c r="I34" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A35" s="17">
+        <f t="shared" si="0"/>
+        <v>27</v>
+      </c>
+      <c r="B35" s="91" t="s">
+        <v>47</v>
+      </c>
+      <c r="C35" s="92"/>
+      <c r="D35" s="93"/>
+      <c r="E35" s="15" t="s">
+        <v>5</v>
+      </c>
+      <c r="F35" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G35" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H35" s="10"/>
+      <c r="I35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A36" s="17">
+        <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="H33" s="10"/>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A34" s="18">
-        <f t="shared" si="0"/>
+      <c r="B36" s="91" t="s">
+        <v>49</v>
+      </c>
+      <c r="C36" s="92"/>
+      <c r="D36" s="93"/>
+      <c r="E36" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F36" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G36" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H36" s="10"/>
+    </row>
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A37" s="17">
+        <f t="shared" si="0"/>
+        <v>29</v>
+      </c>
+      <c r="B37" s="91" t="s">
+        <v>50</v>
+      </c>
+      <c r="C37" s="92"/>
+      <c r="D37" s="93"/>
+      <c r="E37" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F37" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G37" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H37" s="10"/>
+    </row>
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A38" s="17">
+        <f t="shared" si="0"/>
+        <v>30</v>
+      </c>
+      <c r="B38" s="91" t="s">
+        <v>51</v>
+      </c>
+      <c r="C38" s="92"/>
+      <c r="D38" s="93"/>
+      <c r="E38" s="43" t="s">
         <v>26</v>
       </c>
-      <c r="B34" s="130" t="s">
-        <v>49</v>
-      </c>
-      <c r="C34" s="131"/>
-      <c r="D34" s="132"/>
-      <c r="E34" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="F34" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G34" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="H34" s="10"/>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" s="18">
-        <f t="shared" si="0"/>
+      <c r="F38" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G38" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="B35" s="130" t="s">
-        <v>48</v>
-      </c>
-      <c r="C35" s="131"/>
-      <c r="D35" s="132"/>
-      <c r="E35" s="40" t="s">
-        <v>5</v>
-      </c>
-      <c r="F35" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G35" s="37" t="s">
-        <v>28</v>
-      </c>
-      <c r="H35" s="10"/>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" s="18">
-        <f t="shared" si="0"/>
-        <v>28</v>
-      </c>
-      <c r="B36" s="98" t="s">
-        <v>50</v>
-      </c>
-      <c r="C36" s="99"/>
-      <c r="D36" s="100"/>
-      <c r="E36" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F36" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G36" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H36" s="10"/>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" s="18">
-        <f t="shared" si="0"/>
-        <v>29</v>
-      </c>
-      <c r="B37" s="98" t="s">
-        <v>51</v>
-      </c>
-      <c r="C37" s="99"/>
-      <c r="D37" s="100"/>
-      <c r="E37" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F37" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G37" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H37" s="10"/>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" s="18">
-        <f t="shared" si="0"/>
-        <v>30</v>
-      </c>
-      <c r="B38" s="98" t="s">
+      <c r="H38" s="10"/>
+    </row>
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A39" s="17">
+        <f t="shared" si="0"/>
+        <v>31</v>
+      </c>
+      <c r="B39" s="91" t="s">
         <v>52</v>
       </c>
-      <c r="C38" s="99"/>
-      <c r="D38" s="100"/>
-      <c r="E38" s="51" t="s">
+      <c r="C39" s="92"/>
+      <c r="D39" s="93"/>
+      <c r="E39" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F39" s="22" t="s">
+        <v>68</v>
+      </c>
+      <c r="G39" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F38" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G38" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H38" s="10"/>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" s="18">
-        <f t="shared" si="0"/>
-        <v>31</v>
-      </c>
-      <c r="B39" s="98" t="s">
-        <v>53</v>
-      </c>
-      <c r="C39" s="99"/>
-      <c r="D39" s="100"/>
-      <c r="E39" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="F39" s="24" t="s">
-        <v>69</v>
-      </c>
-      <c r="G39" s="52" t="s">
-        <v>28</v>
-      </c>
       <c r="H39" s="10"/>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" s="18">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A40" s="17">
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B40" s="118"/>
-      <c r="C40" s="119"/>
-      <c r="D40" s="120"/>
+      <c r="B40" s="108"/>
+      <c r="C40" s="109"/>
+      <c r="D40" s="110"/>
       <c r="E40" s="8"/>
-      <c r="F40" s="29"/>
-      <c r="G40" s="29"/>
+      <c r="F40" s="26"/>
+      <c r="G40" s="26"/>
       <c r="H40" s="10"/>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" s="18">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A41" s="17">
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B41" s="92" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="93"/>
-      <c r="D41" s="94"/>
-      <c r="E41" s="50" t="s">
+      <c r="B41" s="60" t="s">
+        <v>76</v>
+      </c>
+      <c r="C41" s="61"/>
+      <c r="D41" s="62"/>
+      <c r="E41" s="43" t="s">
         <v>3</v>
       </c>
-      <c r="F41" s="25" t="s">
-        <v>16</v>
-      </c>
-      <c r="G41" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H41" s="10"/>
-    </row>
-    <row r="42" spans="1:8" ht="33" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A42" s="18">
+      <c r="F41" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G41" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H41" s="43" t="s">
+        <v>7</v>
+      </c>
+      <c r="I41" s="59" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="42" spans="1:9" ht="33" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A42" s="17">
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B42" s="80"/>
-      <c r="C42" s="81"/>
-      <c r="D42" s="82"/>
+      <c r="B42" s="79"/>
+      <c r="C42" s="80"/>
+      <c r="D42" s="81"/>
       <c r="E42" s="8"/>
-      <c r="F42" s="29"/>
-      <c r="G42" s="29"/>
+      <c r="F42" s="26"/>
+      <c r="G42" s="26"/>
       <c r="H42" s="10"/>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A43" s="18">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A43" s="17">
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B43" s="89"/>
-      <c r="C43" s="90"/>
-      <c r="D43" s="91"/>
+      <c r="B43" s="85"/>
+      <c r="C43" s="86"/>
+      <c r="D43" s="87"/>
       <c r="E43" s="7"/>
-      <c r="F43" s="29"/>
-      <c r="G43" s="29"/>
+      <c r="F43" s="26"/>
+      <c r="G43" s="26"/>
       <c r="H43" s="10"/>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A44" s="18">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A44" s="17">
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B44" s="86" t="s">
-        <v>20</v>
-      </c>
-      <c r="C44" s="87"/>
-      <c r="D44" s="88"/>
-      <c r="E44" s="56"/>
-      <c r="F44" s="28" t="s">
+      <c r="B44" s="76" t="s">
+        <v>19</v>
+      </c>
+      <c r="C44" s="77"/>
+      <c r="D44" s="78"/>
+      <c r="E44" s="47"/>
+      <c r="F44" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G44" s="54" t="s">
-        <v>45</v>
+      <c r="G44" s="46" t="s">
+        <v>44</v>
       </c>
       <c r="H44" s="10"/>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A45" s="18">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A45" s="17">
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B45" s="74" t="s">
-        <v>26</v>
-      </c>
-      <c r="C45" s="75"/>
-      <c r="D45" s="76"/>
+      <c r="B45" s="70" t="s">
+        <v>25</v>
+      </c>
+      <c r="C45" s="71"/>
+      <c r="D45" s="72"/>
       <c r="E45" s="7"/>
-      <c r="F45" s="27"/>
-      <c r="G45" s="29"/>
+      <c r="F45" s="24"/>
+      <c r="G45" s="26"/>
       <c r="H45" s="10"/>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A46" s="18">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A46" s="17">
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B46" s="68" t="s">
-        <v>34</v>
-      </c>
-      <c r="C46" s="69"/>
-      <c r="D46" s="70"/>
+      <c r="B46" s="60" t="s">
+        <v>33</v>
+      </c>
+      <c r="C46" s="61"/>
+      <c r="D46" s="62"/>
       <c r="E46" s="15" t="s">
         <v>5</v>
       </c>
-      <c r="F46" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G46" s="52" t="s">
-        <v>21</v>
+      <c r="F46" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G46" s="44" t="s">
+        <v>20</v>
       </c>
       <c r="H46" s="10"/>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A47" s="18">
+      <c r="I46" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A47" s="17">
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B47" s="118"/>
-      <c r="C47" s="119"/>
-      <c r="D47" s="120"/>
+      <c r="B47" s="108"/>
+      <c r="C47" s="109"/>
+      <c r="D47" s="110"/>
       <c r="E47" s="13"/>
-      <c r="F47" s="30"/>
-      <c r="G47" s="36"/>
+      <c r="F47" s="27"/>
+      <c r="G47" s="33"/>
       <c r="H47" s="10"/>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A48" s="18">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A48" s="17">
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B48" s="118"/>
-      <c r="C48" s="119"/>
-      <c r="D48" s="120"/>
+      <c r="B48" s="108"/>
+      <c r="C48" s="109"/>
+      <c r="D48" s="110"/>
       <c r="E48" s="13"/>
-      <c r="F48" s="30"/>
-      <c r="G48" s="36"/>
+      <c r="F48" s="27"/>
+      <c r="G48" s="33"/>
       <c r="H48" s="10"/>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A49" s="18">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A49" s="17">
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B49" s="118"/>
-      <c r="C49" s="119"/>
-      <c r="D49" s="120"/>
+      <c r="B49" s="108"/>
+      <c r="C49" s="109"/>
+      <c r="D49" s="110"/>
       <c r="E49" s="13"/>
-      <c r="F49" s="30"/>
-      <c r="G49" s="36"/>
+      <c r="F49" s="27"/>
+      <c r="G49" s="33"/>
       <c r="H49" s="10"/>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A50" s="18">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A50" s="17">
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B50" s="118"/>
-      <c r="C50" s="119"/>
-      <c r="D50" s="120"/>
+      <c r="B50" s="108"/>
+      <c r="C50" s="109"/>
+      <c r="D50" s="110"/>
       <c r="E50" s="13"/>
-      <c r="F50" s="30"/>
-      <c r="G50" s="36"/>
+      <c r="F50" s="27"/>
+      <c r="G50" s="33"/>
       <c r="H50" s="10"/>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A51" s="18">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A51" s="17">
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B51" s="68" t="s">
-        <v>59</v>
-      </c>
-      <c r="C51" s="69"/>
-      <c r="D51" s="70"/>
+      <c r="B51" s="60" t="s">
+        <v>58</v>
+      </c>
+      <c r="C51" s="61"/>
+      <c r="D51" s="62"/>
       <c r="E51" s="12" t="s">
         <v>2</v>
       </c>
-      <c r="F51" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G51" s="52" t="s">
+      <c r="F51" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G51" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H51" s="10"/>
+    </row>
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A52" s="17">
+        <f t="shared" si="0"/>
+        <v>44</v>
+      </c>
+      <c r="B52" s="60" t="s">
         <v>21</v>
       </c>
-      <c r="H51" s="10"/>
-    </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A52" s="18">
-        <f t="shared" si="0"/>
-        <v>44</v>
-      </c>
-      <c r="B52" s="68" t="s">
-        <v>22</v>
-      </c>
-      <c r="C52" s="69"/>
-      <c r="D52" s="70"/>
+      <c r="C52" s="61"/>
+      <c r="D52" s="62"/>
       <c r="E52" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="F52" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G52" s="37" t="s">
-        <v>21</v>
-      </c>
-      <c r="H52" s="34" t="s">
+      <c r="F52" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G52" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H52" s="31" t="s">
+        <v>80</v>
+      </c>
+      <c r="I52" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A53" s="17">
+        <f t="shared" si="0"/>
+        <v>45</v>
+      </c>
+      <c r="B53" s="73"/>
+      <c r="C53" s="74"/>
+      <c r="D53" s="75"/>
+      <c r="E53" s="8"/>
+      <c r="F53" s="26"/>
+      <c r="G53" s="26"/>
+      <c r="H53" s="10"/>
+    </row>
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A54" s="17">
+        <f t="shared" si="0"/>
+        <v>46</v>
+      </c>
+      <c r="B54" s="82" t="s">
+        <v>79</v>
+      </c>
+      <c r="C54" s="83"/>
+      <c r="D54" s="84"/>
+      <c r="E54" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F54" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G54" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H54" s="10" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="55" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A55" s="17">
+        <f t="shared" si="0"/>
+        <v>47</v>
+      </c>
+      <c r="B55" s="111" t="s">
+        <v>70</v>
+      </c>
+      <c r="C55" s="112"/>
+      <c r="D55" s="113"/>
+      <c r="E55" s="49" t="s">
+        <v>2</v>
+      </c>
+      <c r="F55" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G55" s="50" t="s">
+        <v>44</v>
+      </c>
+      <c r="H55" s="10"/>
+    </row>
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A56" s="17">
+        <f t="shared" si="0"/>
+        <v>48</v>
+      </c>
+      <c r="B56" s="82" t="s">
         <v>71</v>
       </c>
-    </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A53" s="18">
-        <f t="shared" si="0"/>
-        <v>45</v>
-      </c>
-      <c r="B53" s="77"/>
-      <c r="C53" s="78"/>
-      <c r="D53" s="79"/>
-      <c r="E53" s="8"/>
-      <c r="F53" s="29"/>
-      <c r="G53" s="29"/>
-      <c r="H53" s="10"/>
-    </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A54" s="18">
-        <f t="shared" si="0"/>
-        <v>46</v>
-      </c>
-      <c r="B54" s="124" t="s">
-        <v>81</v>
-      </c>
-      <c r="C54" s="125"/>
-      <c r="D54" s="126"/>
-      <c r="E54" s="55"/>
-      <c r="F54" s="28" t="s">
-        <v>14</v>
-      </c>
-      <c r="G54" s="54" t="s">
-        <v>79</v>
-      </c>
-      <c r="H54" s="10"/>
-    </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A55" s="18">
-        <f t="shared" si="0"/>
-        <v>47</v>
-      </c>
-      <c r="B55" s="127" t="s">
-        <v>72</v>
-      </c>
-      <c r="C55" s="128"/>
-      <c r="D55" s="129"/>
-      <c r="E55" s="58" t="s">
-        <v>2</v>
-      </c>
-      <c r="F55" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G55" s="59" t="s">
-        <v>45</v>
-      </c>
-      <c r="H55" s="10"/>
-    </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A56" s="18">
-        <f t="shared" si="0"/>
-        <v>48</v>
-      </c>
-      <c r="B56" s="83" t="s">
-        <v>73</v>
-      </c>
-      <c r="C56" s="84"/>
-      <c r="D56" s="85"/>
-      <c r="E56" s="51" t="s">
-        <v>27</v>
-      </c>
-      <c r="F56" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G56" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="H56" s="57"/>
-    </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A57" s="18">
+      <c r="C56" s="83"/>
+      <c r="D56" s="84"/>
+      <c r="E56" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F56" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G56" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="H56" s="48"/>
+    </row>
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A57" s="17">
         <f t="shared" ref="A57:A59" si="1">A53+1</f>
         <v>46</v>
       </c>
-      <c r="B57" s="83" t="s">
-        <v>74</v>
-      </c>
-      <c r="C57" s="84"/>
-      <c r="D57" s="85"/>
-      <c r="E57" s="51" t="s">
+      <c r="B57" s="82" t="s">
+        <v>72</v>
+      </c>
+      <c r="C57" s="83"/>
+      <c r="D57" s="84"/>
+      <c r="E57" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F57" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G57" s="52" t="s">
-        <v>45</v>
+      <c r="F57" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G57" s="44" t="s">
+        <v>44</v>
       </c>
       <c r="H57" s="10"/>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A58" s="18">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A58" s="17">
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B58" s="83" t="s">
-        <v>75</v>
-      </c>
-      <c r="C58" s="84"/>
-      <c r="D58" s="85"/>
-      <c r="E58" s="51" t="s">
+      <c r="B58" s="82" t="s">
+        <v>73</v>
+      </c>
+      <c r="C58" s="83"/>
+      <c r="D58" s="84"/>
+      <c r="E58" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F58" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G58" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="H58" s="57"/>
-    </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A59" s="18">
+      <c r="F58" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G58" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="H58" s="48"/>
+    </row>
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A59" s="17">
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B59" s="127" t="s">
-        <v>76</v>
-      </c>
-      <c r="C59" s="128"/>
-      <c r="D59" s="129"/>
-      <c r="E59" s="58" t="s">
+      <c r="B59" s="111" t="s">
+        <v>74</v>
+      </c>
+      <c r="C59" s="112"/>
+      <c r="D59" s="113"/>
+      <c r="E59" s="49" t="s">
         <v>2</v>
       </c>
-      <c r="F59" s="26" t="s">
-        <v>15</v>
-      </c>
-      <c r="G59" s="59" t="s">
-        <v>45</v>
+      <c r="F59" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="G59" s="50" t="s">
+        <v>44</v>
       </c>
       <c r="H59" s="10"/>
     </row>
-    <row r="60" spans="1:8" ht="60" x14ac:dyDescent="0.25">
-      <c r="A60" s="18">
+    <row r="60" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+      <c r="A60" s="17">
         <f>A56+1</f>
         <v>49</v>
       </c>
-      <c r="B60" s="121" t="s">
+      <c r="B60" s="82" t="s">
+        <v>75</v>
+      </c>
+      <c r="C60" s="83"/>
+      <c r="D60" s="84"/>
+      <c r="E60" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F60" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G60" s="44" t="s">
         <v>77</v>
       </c>
-      <c r="C60" s="122"/>
-      <c r="D60" s="123"/>
-      <c r="E60" s="50" t="s">
-        <v>2</v>
-      </c>
-      <c r="F60" s="25" t="s">
-        <v>14</v>
-      </c>
-      <c r="G60" s="37" t="s">
-        <v>79</v>
-      </c>
-      <c r="H60" s="63" t="s">
-        <v>80</v>
-      </c>
-    </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A61" s="18">
+      <c r="H60" s="54" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A61" s="17">
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B61" s="77"/>
-      <c r="C61" s="78"/>
-      <c r="D61" s="79"/>
+      <c r="B61" s="73"/>
+      <c r="C61" s="74"/>
+      <c r="D61" s="75"/>
       <c r="E61" s="8"/>
-      <c r="F61" s="29"/>
-      <c r="G61" s="29"/>
+      <c r="F61" s="26"/>
+      <c r="G61" s="26"/>
       <c r="H61" s="10"/>
     </row>
-    <row r="62" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A62" s="18">
+    <row r="62" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A62" s="17">
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B62" s="77" t="s">
-        <v>57</v>
-      </c>
-      <c r="C62" s="78"/>
-      <c r="D62" s="79"/>
+      <c r="B62" s="73" t="s">
+        <v>56</v>
+      </c>
+      <c r="C62" s="74"/>
+      <c r="D62" s="75"/>
       <c r="E62" s="8"/>
-      <c r="F62" s="29"/>
-      <c r="G62" s="29" t="s">
-        <v>21</v>
+      <c r="F62" s="26"/>
+      <c r="G62" s="26" t="s">
+        <v>20</v>
       </c>
       <c r="H62" s="10"/>
     </row>
-    <row r="63" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="18">
+    <row r="63" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A63" s="17">
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B63" s="68" t="s">
-        <v>35</v>
-      </c>
-      <c r="C63" s="69"/>
-      <c r="D63" s="70"/>
+      <c r="B63" s="60" t="s">
+        <v>34</v>
+      </c>
+      <c r="C63" s="61"/>
+      <c r="D63" s="62"/>
       <c r="E63" s="15" t="s">
         <v>2</v>
       </c>
-      <c r="F63" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G63" s="52" t="s">
-        <v>21</v>
-      </c>
-      <c r="H63" s="20"/>
-    </row>
-    <row r="64" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A64" s="18">
+      <c r="F63" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G63" s="44" t="s">
+        <v>20</v>
+      </c>
+      <c r="H63" s="19"/>
+    </row>
+    <row r="64" spans="1:9" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A64" s="17">
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B64" s="68" t="s">
+      <c r="B64" s="60" t="s">
+        <v>55</v>
+      </c>
+      <c r="C64" s="61"/>
+      <c r="D64" s="62"/>
+      <c r="E64" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F64" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G64" s="44" t="s">
+        <v>44</v>
+      </c>
+      <c r="H64" s="19"/>
+    </row>
+    <row r="65" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A65" s="17">
+        <f t="shared" si="0"/>
+        <v>54</v>
+      </c>
+      <c r="B65" s="60" t="s">
+        <v>25</v>
+      </c>
+      <c r="C65" s="61"/>
+      <c r="D65" s="62"/>
+      <c r="E65" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F65" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G65" s="44" t="s">
+        <v>77</v>
+      </c>
+      <c r="H65" s="19"/>
+    </row>
+    <row r="66" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A66" s="17">
+        <f t="shared" si="0"/>
+        <v>55</v>
+      </c>
+      <c r="B66" s="60" t="s">
+        <v>35</v>
+      </c>
+      <c r="C66" s="61"/>
+      <c r="D66" s="62"/>
+      <c r="E66" s="43" t="s">
+        <v>2</v>
+      </c>
+      <c r="F66" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G66" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H66" s="19"/>
+    </row>
+    <row r="67" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A67" s="17">
+        <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="C64" s="69"/>
-      <c r="D64" s="70"/>
-      <c r="E64" s="51" t="s">
+      <c r="B67" s="60" t="s">
+        <v>36</v>
+      </c>
+      <c r="C67" s="61"/>
+      <c r="D67" s="62"/>
+      <c r="E67" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F64" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G64" s="52" t="s">
-        <v>45</v>
-      </c>
-      <c r="H64" s="20"/>
-    </row>
-    <row r="65" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A65" s="18">
-        <f t="shared" si="0"/>
-        <v>54</v>
-      </c>
-      <c r="B65" s="68" t="s">
-        <v>36</v>
-      </c>
-      <c r="C65" s="69"/>
-      <c r="D65" s="70"/>
-      <c r="E65" s="51" t="s">
+      <c r="F67" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G67" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H67" s="19"/>
+    </row>
+    <row r="68" spans="1:8" s="16" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A68" s="17">
+        <f>A67+1</f>
+        <v>57</v>
+      </c>
+      <c r="B68" s="60" t="s">
+        <v>41</v>
+      </c>
+      <c r="C68" s="61"/>
+      <c r="D68" s="62"/>
+      <c r="E68" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F65" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G65" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H65" s="20"/>
-    </row>
-    <row r="66" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A66" s="18">
-        <f t="shared" si="0"/>
-        <v>55</v>
-      </c>
-      <c r="B66" s="68" t="s">
-        <v>37</v>
-      </c>
-      <c r="C66" s="69"/>
-      <c r="D66" s="70"/>
-      <c r="E66" s="51" t="s">
+      <c r="F68" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G68" s="44" t="s">
+        <v>27</v>
+      </c>
+      <c r="H68" s="19"/>
+    </row>
+    <row r="69" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A69" s="17">
+        <f t="shared" si="0"/>
+        <v>58</v>
+      </c>
+      <c r="B69" s="60" t="s">
+        <v>42</v>
+      </c>
+      <c r="C69" s="61"/>
+      <c r="D69" s="62"/>
+      <c r="E69" s="43" t="s">
+        <v>26</v>
+      </c>
+      <c r="F69" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G69" s="44" t="s">
+        <v>22</v>
+      </c>
+      <c r="H69" s="45" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A70" s="17">
+        <f t="shared" si="0"/>
+        <v>59</v>
+      </c>
+      <c r="B70" s="60" t="s">
+        <v>43</v>
+      </c>
+      <c r="C70" s="61"/>
+      <c r="D70" s="62"/>
+      <c r="E70" s="43" t="s">
         <v>2</v>
       </c>
-      <c r="F66" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G66" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H66" s="20"/>
-    </row>
-    <row r="67" spans="1:8" s="17" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A67" s="18">
-        <f t="shared" si="0"/>
-        <v>56</v>
-      </c>
-      <c r="B67" s="68" t="s">
-        <v>42</v>
-      </c>
-      <c r="C67" s="69"/>
-      <c r="D67" s="70"/>
-      <c r="E67" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F67" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G67" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H67" s="20"/>
-    </row>
-    <row r="68" spans="1:8" ht="44.25" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A68" s="18">
-        <f t="shared" si="0"/>
-        <v>57</v>
-      </c>
-      <c r="B68" s="68" t="s">
-        <v>43</v>
-      </c>
-      <c r="C68" s="69"/>
-      <c r="D68" s="70"/>
-      <c r="E68" s="51" t="s">
+      <c r="F70" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="G70" s="44" t="s">
         <v>27</v>
       </c>
-      <c r="F68" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G68" s="52" t="s">
-        <v>23</v>
-      </c>
-      <c r="H68" s="53" t="s">
-        <v>70</v>
-      </c>
-    </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A69" s="18">
-        <f t="shared" si="0"/>
-        <v>58</v>
-      </c>
-      <c r="B69" s="68" t="s">
-        <v>44</v>
-      </c>
-      <c r="C69" s="69"/>
-      <c r="D69" s="70"/>
-      <c r="E69" s="51" t="s">
-        <v>2</v>
-      </c>
-      <c r="F69" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="G69" s="52" t="s">
-        <v>28</v>
-      </c>
-      <c r="H69" s="10"/>
-    </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A70" s="18">
-        <f t="shared" si="0"/>
-        <v>59</v>
-      </c>
-      <c r="B70" s="80"/>
-      <c r="C70" s="81"/>
-      <c r="D70" s="82"/>
-      <c r="E70" s="8"/>
-      <c r="F70" s="29"/>
-      <c r="G70" s="29"/>
       <c r="H70" s="10"/>
     </row>
     <row r="71" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A71" s="18">
+      <c r="A71" s="17">
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B71" s="80"/>
-      <c r="C71" s="81"/>
-      <c r="D71" s="82"/>
+      <c r="B71" s="79"/>
+      <c r="C71" s="80"/>
+      <c r="D71" s="81"/>
       <c r="E71" s="8"/>
-      <c r="F71" s="29"/>
-      <c r="G71" s="29"/>
+      <c r="F71" s="26"/>
+      <c r="G71" s="26"/>
       <c r="H71" s="10"/>
     </row>
     <row r="72" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A72" s="18">
+      <c r="A72" s="17">
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B72" s="80" t="s">
-        <v>25</v>
-      </c>
-      <c r="C72" s="81"/>
-      <c r="D72" s="82"/>
-      <c r="E72" s="13"/>
-      <c r="F72" s="28" t="s">
+      <c r="B72" s="79"/>
+      <c r="C72" s="80"/>
+      <c r="D72" s="81"/>
+      <c r="E72" s="8"/>
+      <c r="F72" s="26"/>
+      <c r="G72" s="26"/>
+      <c r="H72" s="10"/>
+    </row>
+    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A73" s="17">
+        <f t="shared" si="0"/>
+        <v>62</v>
+      </c>
+      <c r="B73" s="76" t="s">
+        <v>24</v>
+      </c>
+      <c r="C73" s="77"/>
+      <c r="D73" s="78"/>
+      <c r="E73" s="58"/>
+      <c r="F73" s="25" t="s">
         <v>14</v>
       </c>
-      <c r="G72" s="29" t="s">
+      <c r="G73" s="26" t="s">
+        <v>61</v>
+      </c>
+      <c r="H73" s="10" t="s">
         <v>62</v>
       </c>
-      <c r="H72" s="10" t="s">
+    </row>
+    <row r="74" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="17">
+        <f t="shared" si="0"/>
         <v>63</v>
       </c>
-    </row>
-    <row r="73" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A73" s="18">
-        <f t="shared" si="0"/>
-        <v>62</v>
-      </c>
-      <c r="B73" s="71"/>
-      <c r="C73" s="72"/>
-      <c r="D73" s="73"/>
-      <c r="E73" s="9"/>
-      <c r="F73" s="31"/>
-      <c r="G73" s="31"/>
-      <c r="H73" s="11"/>
+      <c r="B74" s="67"/>
+      <c r="C74" s="68"/>
+      <c r="D74" s="69"/>
+      <c r="E74" s="9"/>
+      <c r="F74" s="28"/>
+      <c r="G74" s="28"/>
+      <c r="H74" s="11"/>
     </row>
   </sheetData>
-  <mergeCells count="66">
-    <mergeCell ref="B33:D33"/>
+  <mergeCells count="67">
     <mergeCell ref="B34:D34"/>
     <mergeCell ref="B35:D35"/>
     <mergeCell ref="B36:D36"/>
     <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B40:D40"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="B60:D60"/>
     <mergeCell ref="B61:D61"/>
@@ -2681,26 +2674,17 @@
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="B59:D59"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B33:D33"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
     <mergeCell ref="B2:D2"/>
     <mergeCell ref="B10:D10"/>
     <mergeCell ref="B11:D11"/>
     <mergeCell ref="B13:D13"/>
     <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B32:D32"/>
-    <mergeCell ref="B40:D40"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B69:D69"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B44:D44"/>
     <mergeCell ref="B16:D16"/>
     <mergeCell ref="B43:D43"/>
     <mergeCell ref="B20:D20"/>
@@ -2713,22 +2697,31 @@
     <mergeCell ref="B41:D41"/>
     <mergeCell ref="B24:D24"/>
     <mergeCell ref="B26:D26"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B65:D65"/>
     <mergeCell ref="H10:H11"/>
     <mergeCell ref="E10:E11"/>
     <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B74:D74"/>
     <mergeCell ref="B45:D45"/>
     <mergeCell ref="B46:D46"/>
     <mergeCell ref="B51:D51"/>
     <mergeCell ref="B52:D52"/>
     <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="B63:D63"/>
     <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B69:D69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>

<commit_message>
Apresentação final e atualizações de ficheiros no repositório, e acição de comentários em algumas partes do código da app
</commit_message>
<xml_diff>
--- a/6OrganiçaoGrupo(Importante)/Tarefas_app.xlsx
+++ b/6OrganiçaoGrupo(Importante)/Tarefas_app.xlsx
@@ -812,6 +812,24 @@
     </xf>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="1" fillId="5" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
@@ -819,6 +837,120 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="30" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -840,138 +972,6 @@
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="23" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="14" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -1281,7 +1281,7 @@
   <dimension ref="A1:I74"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B10" sqref="B10:D10"/>
+      <selection activeCell="B52" sqref="B52:D52"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1297,11 +1297,11 @@
   <sheetData>
     <row r="1" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3"/>
     <row r="2" spans="1:8" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B2" s="94" t="s">
+      <c r="B2" s="90" t="s">
         <v>0</v>
       </c>
-      <c r="C2" s="95"/>
-      <c r="D2" s="95"/>
+      <c r="C2" s="91"/>
+      <c r="D2" s="91"/>
       <c r="E2" s="6" t="s">
         <v>1</v>
       </c>
@@ -1373,11 +1373,11 @@
       <c r="A9" s="17">
         <v>1</v>
       </c>
-      <c r="B9" s="60" t="s">
+      <c r="B9" s="66" t="s">
         <v>11</v>
       </c>
-      <c r="C9" s="61"/>
-      <c r="D9" s="62"/>
+      <c r="C9" s="67"/>
+      <c r="D9" s="68"/>
       <c r="E9" s="14" t="s">
         <v>2</v>
       </c>
@@ -1394,12 +1394,12 @@
         <f>A9+1</f>
         <v>2</v>
       </c>
-      <c r="B10" s="96" t="s">
+      <c r="B10" s="92" t="s">
         <v>8</v>
       </c>
-      <c r="C10" s="97"/>
-      <c r="D10" s="98"/>
-      <c r="E10" s="65" t="s">
+      <c r="C10" s="93"/>
+      <c r="D10" s="94"/>
+      <c r="E10" s="109" t="s">
         <v>63</v>
       </c>
       <c r="F10" s="22" t="s">
@@ -1408,7 +1408,7 @@
       <c r="G10" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H10" s="63" t="s">
+      <c r="H10" s="107" t="s">
         <v>23</v>
       </c>
     </row>
@@ -1417,30 +1417,30 @@
         <f t="shared" ref="A11:A74" si="0">A10+1</f>
         <v>3</v>
       </c>
-      <c r="B11" s="60" t="s">
+      <c r="B11" s="66" t="s">
         <v>9</v>
       </c>
-      <c r="C11" s="61"/>
-      <c r="D11" s="62"/>
-      <c r="E11" s="66"/>
+      <c r="C11" s="67"/>
+      <c r="D11" s="68"/>
+      <c r="E11" s="110"/>
       <c r="F11" s="22" t="s">
         <v>15</v>
       </c>
       <c r="G11" s="26" t="s">
         <v>22</v>
       </c>
-      <c r="H11" s="64"/>
+      <c r="H11" s="108"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A12" s="17">
         <f t="shared" si="0"/>
         <v>4</v>
       </c>
-      <c r="B12" s="60" t="s">
+      <c r="B12" s="66" t="s">
         <v>16</v>
       </c>
-      <c r="C12" s="61"/>
-      <c r="D12" s="62"/>
+      <c r="C12" s="67"/>
+      <c r="D12" s="68"/>
       <c r="E12" s="12" t="s">
         <v>26</v>
       </c>
@@ -1457,11 +1457,11 @@
         <f t="shared" si="0"/>
         <v>5</v>
       </c>
-      <c r="B13" s="60" t="s">
+      <c r="B13" s="66" t="s">
         <v>28</v>
       </c>
-      <c r="C13" s="61"/>
-      <c r="D13" s="62"/>
+      <c r="C13" s="67"/>
+      <c r="D13" s="68"/>
       <c r="E13" s="14" t="s">
         <v>2</v>
       </c>
@@ -1478,11 +1478,11 @@
         <f t="shared" si="0"/>
         <v>6</v>
       </c>
-      <c r="B14" s="102" t="s">
+      <c r="B14" s="78" t="s">
         <v>38</v>
       </c>
-      <c r="C14" s="103"/>
-      <c r="D14" s="104"/>
+      <c r="C14" s="79"/>
+      <c r="D14" s="80"/>
       <c r="E14" s="14" t="s">
         <v>2</v>
       </c>
@@ -1499,11 +1499,11 @@
         <f t="shared" si="0"/>
         <v>7</v>
       </c>
-      <c r="B15" s="102" t="s">
+      <c r="B15" s="78" t="s">
         <v>37</v>
       </c>
-      <c r="C15" s="103"/>
-      <c r="D15" s="104"/>
+      <c r="C15" s="79"/>
+      <c r="D15" s="80"/>
       <c r="E15" s="14" t="s">
         <v>6</v>
       </c>
@@ -1520,11 +1520,11 @@
         <f t="shared" si="0"/>
         <v>8</v>
       </c>
-      <c r="B16" s="60" t="s">
+      <c r="B16" s="66" t="s">
         <v>29</v>
       </c>
-      <c r="C16" s="61"/>
-      <c r="D16" s="62"/>
+      <c r="C16" s="67"/>
+      <c r="D16" s="68"/>
       <c r="E16" s="14" t="s">
         <v>5</v>
       </c>
@@ -1541,11 +1541,11 @@
         <f t="shared" si="0"/>
         <v>9</v>
       </c>
-      <c r="B17" s="60" t="s">
+      <c r="B17" s="66" t="s">
         <v>30</v>
       </c>
-      <c r="C17" s="61"/>
-      <c r="D17" s="62"/>
+      <c r="C17" s="67"/>
+      <c r="D17" s="68"/>
       <c r="E17" s="14" t="s">
         <v>2</v>
       </c>
@@ -1562,11 +1562,11 @@
         <f t="shared" si="0"/>
         <v>10</v>
       </c>
-      <c r="B18" s="60" t="s">
+      <c r="B18" s="66" t="s">
         <v>31</v>
       </c>
-      <c r="C18" s="61"/>
-      <c r="D18" s="62"/>
+      <c r="C18" s="67"/>
+      <c r="D18" s="68"/>
       <c r="E18" s="14" t="s">
         <v>26</v>
       </c>
@@ -1583,11 +1583,11 @@
         <f t="shared" si="0"/>
         <v>11</v>
       </c>
-      <c r="B19" s="105" t="s">
+      <c r="B19" s="81" t="s">
         <v>39</v>
       </c>
-      <c r="C19" s="106"/>
-      <c r="D19" s="107"/>
+      <c r="C19" s="82"/>
+      <c r="D19" s="83"/>
       <c r="E19" s="18" t="s">
         <v>2</v>
       </c>
@@ -1604,11 +1604,11 @@
         <f t="shared" si="0"/>
         <v>12</v>
       </c>
-      <c r="B20" s="60" t="s">
+      <c r="B20" s="66" t="s">
         <v>12</v>
       </c>
-      <c r="C20" s="61"/>
-      <c r="D20" s="62"/>
+      <c r="C20" s="67"/>
+      <c r="D20" s="68"/>
       <c r="E20" s="12" t="s">
         <v>5</v>
       </c>
@@ -1625,11 +1625,11 @@
         <f t="shared" si="0"/>
         <v>13</v>
       </c>
-      <c r="B21" s="70" t="s">
+      <c r="B21" s="87" t="s">
         <v>32</v>
       </c>
-      <c r="C21" s="71"/>
-      <c r="D21" s="72"/>
+      <c r="C21" s="88"/>
+      <c r="D21" s="89"/>
       <c r="E21" s="7"/>
       <c r="F21" s="24"/>
       <c r="G21" s="26"/>
@@ -1640,11 +1640,11 @@
         <f t="shared" si="0"/>
         <v>14</v>
       </c>
-      <c r="B22" s="60" t="s">
+      <c r="B22" s="66" t="s">
         <v>17</v>
       </c>
-      <c r="C22" s="61"/>
-      <c r="D22" s="62"/>
+      <c r="C22" s="67"/>
+      <c r="D22" s="68"/>
       <c r="E22" s="15" t="s">
         <v>5</v>
       </c>
@@ -1663,11 +1663,11 @@
         <f t="shared" si="0"/>
         <v>15</v>
       </c>
-      <c r="B23" s="60" t="s">
+      <c r="B23" s="66" t="s">
         <v>18</v>
       </c>
-      <c r="C23" s="61"/>
-      <c r="D23" s="62"/>
+      <c r="C23" s="67"/>
+      <c r="D23" s="68"/>
       <c r="E23" s="12" t="s">
         <v>26</v>
       </c>
@@ -1684,11 +1684,11 @@
         <f t="shared" si="0"/>
         <v>16</v>
       </c>
-      <c r="B24" s="60" t="s">
+      <c r="B24" s="66" t="s">
         <v>10</v>
       </c>
-      <c r="C24" s="61"/>
-      <c r="D24" s="62"/>
+      <c r="C24" s="67"/>
+      <c r="D24" s="68"/>
       <c r="E24" s="14" t="s">
         <v>26</v>
       </c>
@@ -1705,11 +1705,11 @@
         <f t="shared" si="0"/>
         <v>17</v>
       </c>
-      <c r="B25" s="60" t="s">
+      <c r="B25" s="66" t="s">
         <v>57</v>
       </c>
-      <c r="C25" s="61"/>
-      <c r="D25" s="62"/>
+      <c r="C25" s="67"/>
+      <c r="D25" s="68"/>
       <c r="E25" s="15" t="s">
         <v>2</v>
       </c>
@@ -1726,11 +1726,11 @@
         <f t="shared" si="0"/>
         <v>18</v>
       </c>
-      <c r="B26" s="88" t="s">
+      <c r="B26" s="98" t="s">
         <v>64</v>
       </c>
-      <c r="C26" s="89"/>
-      <c r="D26" s="90"/>
+      <c r="C26" s="99"/>
+      <c r="D26" s="100"/>
       <c r="E26" s="37" t="s">
         <v>26</v>
       </c>
@@ -1747,11 +1747,11 @@
         <f t="shared" si="0"/>
         <v>19</v>
       </c>
-      <c r="B27" s="99" t="s">
+      <c r="B27" s="101" t="s">
         <v>65</v>
       </c>
-      <c r="C27" s="100"/>
-      <c r="D27" s="101"/>
+      <c r="C27" s="102"/>
+      <c r="D27" s="103"/>
       <c r="E27" s="41" t="s">
         <v>26</v>
       </c>
@@ -1810,9 +1810,9 @@
         <f t="shared" si="0"/>
         <v>22</v>
       </c>
-      <c r="B30" s="79"/>
-      <c r="C30" s="80"/>
-      <c r="D30" s="81"/>
+      <c r="B30" s="84"/>
+      <c r="C30" s="85"/>
+      <c r="D30" s="86"/>
       <c r="E30" s="7"/>
       <c r="F30" s="24"/>
       <c r="G30" s="26"/>
@@ -1823,11 +1823,11 @@
         <f t="shared" si="0"/>
         <v>23</v>
       </c>
-      <c r="B31" s="70" t="s">
+      <c r="B31" s="87" t="s">
         <v>45</v>
       </c>
-      <c r="C31" s="71"/>
-      <c r="D31" s="72"/>
+      <c r="C31" s="88"/>
+      <c r="D31" s="89"/>
       <c r="E31" s="7"/>
       <c r="F31" s="24"/>
       <c r="G31" s="26"/>
@@ -1838,11 +1838,11 @@
         <f t="shared" si="0"/>
         <v>24</v>
       </c>
-      <c r="B32" s="91" t="s">
+      <c r="B32" s="60" t="s">
         <v>53</v>
       </c>
-      <c r="C32" s="92"/>
-      <c r="D32" s="93"/>
+      <c r="C32" s="61"/>
+      <c r="D32" s="62"/>
       <c r="E32" s="14" t="s">
         <v>2</v>
       </c>
@@ -1859,11 +1859,11 @@
         <f t="shared" si="0"/>
         <v>25</v>
       </c>
-      <c r="B33" s="91" t="s">
+      <c r="B33" s="60" t="s">
         <v>54</v>
       </c>
-      <c r="C33" s="92"/>
-      <c r="D33" s="93"/>
+      <c r="C33" s="61"/>
+      <c r="D33" s="62"/>
       <c r="E33" s="14" t="s">
         <v>2</v>
       </c>
@@ -1880,11 +1880,11 @@
         <f t="shared" si="0"/>
         <v>26</v>
       </c>
-      <c r="B34" s="91" t="s">
+      <c r="B34" s="60" t="s">
         <v>48</v>
       </c>
-      <c r="C34" s="92"/>
-      <c r="D34" s="93"/>
+      <c r="C34" s="61"/>
+      <c r="D34" s="62"/>
       <c r="E34" s="15" t="s">
         <v>5</v>
       </c>
@@ -1904,11 +1904,11 @@
         <f t="shared" si="0"/>
         <v>27</v>
       </c>
-      <c r="B35" s="91" t="s">
+      <c r="B35" s="60" t="s">
         <v>47</v>
       </c>
-      <c r="C35" s="92"/>
-      <c r="D35" s="93"/>
+      <c r="C35" s="61"/>
+      <c r="D35" s="62"/>
       <c r="E35" s="15" t="s">
         <v>5</v>
       </c>
@@ -1928,11 +1928,11 @@
         <f t="shared" si="0"/>
         <v>28</v>
       </c>
-      <c r="B36" s="91" t="s">
+      <c r="B36" s="60" t="s">
         <v>49</v>
       </c>
-      <c r="C36" s="92"/>
-      <c r="D36" s="93"/>
+      <c r="C36" s="61"/>
+      <c r="D36" s="62"/>
       <c r="E36" s="43" t="s">
         <v>2</v>
       </c>
@@ -1949,11 +1949,11 @@
         <f t="shared" si="0"/>
         <v>29</v>
       </c>
-      <c r="B37" s="91" t="s">
+      <c r="B37" s="60" t="s">
         <v>50</v>
       </c>
-      <c r="C37" s="92"/>
-      <c r="D37" s="93"/>
+      <c r="C37" s="61"/>
+      <c r="D37" s="62"/>
       <c r="E37" s="43" t="s">
         <v>2</v>
       </c>
@@ -1970,11 +1970,11 @@
         <f t="shared" si="0"/>
         <v>30</v>
       </c>
-      <c r="B38" s="91" t="s">
+      <c r="B38" s="60" t="s">
         <v>51</v>
       </c>
-      <c r="C38" s="92"/>
-      <c r="D38" s="93"/>
+      <c r="C38" s="61"/>
+      <c r="D38" s="62"/>
       <c r="E38" s="43" t="s">
         <v>26</v>
       </c>
@@ -1991,11 +1991,11 @@
         <f t="shared" si="0"/>
         <v>31</v>
       </c>
-      <c r="B39" s="91" t="s">
+      <c r="B39" s="60" t="s">
         <v>52</v>
       </c>
-      <c r="C39" s="92"/>
-      <c r="D39" s="93"/>
+      <c r="C39" s="61"/>
+      <c r="D39" s="62"/>
       <c r="E39" s="43" t="s">
         <v>26</v>
       </c>
@@ -2012,9 +2012,9 @@
         <f t="shared" si="0"/>
         <v>32</v>
       </c>
-      <c r="B40" s="108"/>
-      <c r="C40" s="109"/>
-      <c r="D40" s="110"/>
+      <c r="B40" s="63"/>
+      <c r="C40" s="64"/>
+      <c r="D40" s="65"/>
       <c r="E40" s="8"/>
       <c r="F40" s="26"/>
       <c r="G40" s="26"/>
@@ -2025,11 +2025,11 @@
         <f t="shared" si="0"/>
         <v>33</v>
       </c>
-      <c r="B41" s="60" t="s">
+      <c r="B41" s="66" t="s">
         <v>76</v>
       </c>
-      <c r="C41" s="61"/>
-      <c r="D41" s="62"/>
+      <c r="C41" s="67"/>
+      <c r="D41" s="68"/>
       <c r="E41" s="43" t="s">
         <v>3</v>
       </c>
@@ -2051,9 +2051,9 @@
         <f t="shared" si="0"/>
         <v>34</v>
       </c>
-      <c r="B42" s="79"/>
-      <c r="C42" s="80"/>
-      <c r="D42" s="81"/>
+      <c r="B42" s="84"/>
+      <c r="C42" s="85"/>
+      <c r="D42" s="86"/>
       <c r="E42" s="8"/>
       <c r="F42" s="26"/>
       <c r="G42" s="26"/>
@@ -2064,9 +2064,9 @@
         <f t="shared" si="0"/>
         <v>35</v>
       </c>
-      <c r="B43" s="85"/>
-      <c r="C43" s="86"/>
-      <c r="D43" s="87"/>
+      <c r="B43" s="95"/>
+      <c r="C43" s="96"/>
+      <c r="D43" s="97"/>
       <c r="E43" s="7"/>
       <c r="F43" s="26"/>
       <c r="G43" s="26"/>
@@ -2077,11 +2077,11 @@
         <f t="shared" si="0"/>
         <v>36</v>
       </c>
-      <c r="B44" s="76" t="s">
+      <c r="B44" s="104" t="s">
         <v>19</v>
       </c>
-      <c r="C44" s="77"/>
-      <c r="D44" s="78"/>
+      <c r="C44" s="105"/>
+      <c r="D44" s="106"/>
       <c r="E44" s="47"/>
       <c r="F44" s="25" t="s">
         <v>14</v>
@@ -2096,11 +2096,11 @@
         <f t="shared" si="0"/>
         <v>37</v>
       </c>
-      <c r="B45" s="70" t="s">
+      <c r="B45" s="87" t="s">
         <v>25</v>
       </c>
-      <c r="C45" s="71"/>
-      <c r="D45" s="72"/>
+      <c r="C45" s="88"/>
+      <c r="D45" s="89"/>
       <c r="E45" s="7"/>
       <c r="F45" s="24"/>
       <c r="G45" s="26"/>
@@ -2111,11 +2111,11 @@
         <f t="shared" si="0"/>
         <v>38</v>
       </c>
-      <c r="B46" s="60" t="s">
+      <c r="B46" s="66" t="s">
         <v>33</v>
       </c>
-      <c r="C46" s="61"/>
-      <c r="D46" s="62"/>
+      <c r="C46" s="67"/>
+      <c r="D46" s="68"/>
       <c r="E46" s="15" t="s">
         <v>5</v>
       </c>
@@ -2135,9 +2135,9 @@
         <f t="shared" si="0"/>
         <v>39</v>
       </c>
-      <c r="B47" s="108"/>
-      <c r="C47" s="109"/>
-      <c r="D47" s="110"/>
+      <c r="B47" s="63"/>
+      <c r="C47" s="64"/>
+      <c r="D47" s="65"/>
       <c r="E47" s="13"/>
       <c r="F47" s="27"/>
       <c r="G47" s="33"/>
@@ -2148,9 +2148,9 @@
         <f t="shared" si="0"/>
         <v>40</v>
       </c>
-      <c r="B48" s="108"/>
-      <c r="C48" s="109"/>
-      <c r="D48" s="110"/>
+      <c r="B48" s="63"/>
+      <c r="C48" s="64"/>
+      <c r="D48" s="65"/>
       <c r="E48" s="13"/>
       <c r="F48" s="27"/>
       <c r="G48" s="33"/>
@@ -2161,9 +2161,9 @@
         <f t="shared" si="0"/>
         <v>41</v>
       </c>
-      <c r="B49" s="108"/>
-      <c r="C49" s="109"/>
-      <c r="D49" s="110"/>
+      <c r="B49" s="63"/>
+      <c r="C49" s="64"/>
+      <c r="D49" s="65"/>
       <c r="E49" s="13"/>
       <c r="F49" s="27"/>
       <c r="G49" s="33"/>
@@ -2174,9 +2174,9 @@
         <f t="shared" si="0"/>
         <v>42</v>
       </c>
-      <c r="B50" s="108"/>
-      <c r="C50" s="109"/>
-      <c r="D50" s="110"/>
+      <c r="B50" s="63"/>
+      <c r="C50" s="64"/>
+      <c r="D50" s="65"/>
       <c r="E50" s="13"/>
       <c r="F50" s="27"/>
       <c r="G50" s="33"/>
@@ -2187,11 +2187,11 @@
         <f t="shared" si="0"/>
         <v>43</v>
       </c>
-      <c r="B51" s="60" t="s">
+      <c r="B51" s="66" t="s">
         <v>58</v>
       </c>
-      <c r="C51" s="61"/>
-      <c r="D51" s="62"/>
+      <c r="C51" s="67"/>
+      <c r="D51" s="68"/>
       <c r="E51" s="12" t="s">
         <v>2</v>
       </c>
@@ -2208,11 +2208,11 @@
         <f t="shared" si="0"/>
         <v>44</v>
       </c>
-      <c r="B52" s="60" t="s">
+      <c r="B52" s="66" t="s">
         <v>21</v>
       </c>
-      <c r="C52" s="61"/>
-      <c r="D52" s="62"/>
+      <c r="C52" s="67"/>
+      <c r="D52" s="68"/>
       <c r="E52" s="14" t="s">
         <v>5</v>
       </c>
@@ -2234,9 +2234,9 @@
         <f t="shared" si="0"/>
         <v>45</v>
       </c>
-      <c r="B53" s="73"/>
-      <c r="C53" s="74"/>
-      <c r="D53" s="75"/>
+      <c r="B53" s="72"/>
+      <c r="C53" s="73"/>
+      <c r="D53" s="74"/>
       <c r="E53" s="8"/>
       <c r="F53" s="26"/>
       <c r="G53" s="26"/>
@@ -2247,11 +2247,11 @@
         <f t="shared" si="0"/>
         <v>46</v>
       </c>
-      <c r="B54" s="82" t="s">
+      <c r="B54" s="69" t="s">
         <v>79</v>
       </c>
-      <c r="C54" s="83"/>
-      <c r="D54" s="84"/>
+      <c r="C54" s="70"/>
+      <c r="D54" s="71"/>
       <c r="E54" s="43" t="s">
         <v>26</v>
       </c>
@@ -2270,11 +2270,11 @@
         <f t="shared" si="0"/>
         <v>47</v>
       </c>
-      <c r="B55" s="111" t="s">
+      <c r="B55" s="75" t="s">
         <v>70</v>
       </c>
-      <c r="C55" s="112"/>
-      <c r="D55" s="113"/>
+      <c r="C55" s="76"/>
+      <c r="D55" s="77"/>
       <c r="E55" s="49" t="s">
         <v>2</v>
       </c>
@@ -2291,11 +2291,11 @@
         <f t="shared" si="0"/>
         <v>48</v>
       </c>
-      <c r="B56" s="82" t="s">
+      <c r="B56" s="69" t="s">
         <v>71</v>
       </c>
-      <c r="C56" s="83"/>
-      <c r="D56" s="84"/>
+      <c r="C56" s="70"/>
+      <c r="D56" s="71"/>
       <c r="E56" s="43" t="s">
         <v>26</v>
       </c>
@@ -2312,11 +2312,11 @@
         <f t="shared" ref="A57:A59" si="1">A53+1</f>
         <v>46</v>
       </c>
-      <c r="B57" s="82" t="s">
+      <c r="B57" s="69" t="s">
         <v>72</v>
       </c>
-      <c r="C57" s="83"/>
-      <c r="D57" s="84"/>
+      <c r="C57" s="70"/>
+      <c r="D57" s="71"/>
       <c r="E57" s="43" t="s">
         <v>2</v>
       </c>
@@ -2333,11 +2333,11 @@
         <f t="shared" si="1"/>
         <v>47</v>
       </c>
-      <c r="B58" s="82" t="s">
+      <c r="B58" s="69" t="s">
         <v>73</v>
       </c>
-      <c r="C58" s="83"/>
-      <c r="D58" s="84"/>
+      <c r="C58" s="70"/>
+      <c r="D58" s="71"/>
       <c r="E58" s="43" t="s">
         <v>2</v>
       </c>
@@ -2354,11 +2354,11 @@
         <f t="shared" si="1"/>
         <v>48</v>
       </c>
-      <c r="B59" s="111" t="s">
+      <c r="B59" s="75" t="s">
         <v>74</v>
       </c>
-      <c r="C59" s="112"/>
-      <c r="D59" s="113"/>
+      <c r="C59" s="76"/>
+      <c r="D59" s="77"/>
       <c r="E59" s="49" t="s">
         <v>2</v>
       </c>
@@ -2375,11 +2375,11 @@
         <f>A56+1</f>
         <v>49</v>
       </c>
-      <c r="B60" s="82" t="s">
+      <c r="B60" s="69" t="s">
         <v>75</v>
       </c>
-      <c r="C60" s="83"/>
-      <c r="D60" s="84"/>
+      <c r="C60" s="70"/>
+      <c r="D60" s="71"/>
       <c r="E60" s="43" t="s">
         <v>2</v>
       </c>
@@ -2398,9 +2398,9 @@
         <f t="shared" si="0"/>
         <v>50</v>
       </c>
-      <c r="B61" s="73"/>
-      <c r="C61" s="74"/>
-      <c r="D61" s="75"/>
+      <c r="B61" s="72"/>
+      <c r="C61" s="73"/>
+      <c r="D61" s="74"/>
       <c r="E61" s="8"/>
       <c r="F61" s="26"/>
       <c r="G61" s="26"/>
@@ -2411,11 +2411,11 @@
         <f t="shared" si="0"/>
         <v>51</v>
       </c>
-      <c r="B62" s="73" t="s">
+      <c r="B62" s="72" t="s">
         <v>56</v>
       </c>
-      <c r="C62" s="74"/>
-      <c r="D62" s="75"/>
+      <c r="C62" s="73"/>
+      <c r="D62" s="74"/>
       <c r="E62" s="8"/>
       <c r="F62" s="26"/>
       <c r="G62" s="26" t="s">
@@ -2428,11 +2428,11 @@
         <f t="shared" si="0"/>
         <v>52</v>
       </c>
-      <c r="B63" s="60" t="s">
+      <c r="B63" s="66" t="s">
         <v>34</v>
       </c>
-      <c r="C63" s="61"/>
-      <c r="D63" s="62"/>
+      <c r="C63" s="67"/>
+      <c r="D63" s="68"/>
       <c r="E63" s="15" t="s">
         <v>2</v>
       </c>
@@ -2449,11 +2449,11 @@
         <f t="shared" si="0"/>
         <v>53</v>
       </c>
-      <c r="B64" s="60" t="s">
+      <c r="B64" s="66" t="s">
         <v>55</v>
       </c>
-      <c r="C64" s="61"/>
-      <c r="D64" s="62"/>
+      <c r="C64" s="67"/>
+      <c r="D64" s="68"/>
       <c r="E64" s="43" t="s">
         <v>2</v>
       </c>
@@ -2470,11 +2470,11 @@
         <f t="shared" si="0"/>
         <v>54</v>
       </c>
-      <c r="B65" s="60" t="s">
+      <c r="B65" s="66" t="s">
         <v>25</v>
       </c>
-      <c r="C65" s="61"/>
-      <c r="D65" s="62"/>
+      <c r="C65" s="67"/>
+      <c r="D65" s="68"/>
       <c r="E65" s="43" t="s">
         <v>2</v>
       </c>
@@ -2491,11 +2491,11 @@
         <f t="shared" si="0"/>
         <v>55</v>
       </c>
-      <c r="B66" s="60" t="s">
+      <c r="B66" s="66" t="s">
         <v>35</v>
       </c>
-      <c r="C66" s="61"/>
-      <c r="D66" s="62"/>
+      <c r="C66" s="67"/>
+      <c r="D66" s="68"/>
       <c r="E66" s="43" t="s">
         <v>2</v>
       </c>
@@ -2512,11 +2512,11 @@
         <f t="shared" si="0"/>
         <v>56</v>
       </c>
-      <c r="B67" s="60" t="s">
+      <c r="B67" s="66" t="s">
         <v>36</v>
       </c>
-      <c r="C67" s="61"/>
-      <c r="D67" s="62"/>
+      <c r="C67" s="67"/>
+      <c r="D67" s="68"/>
       <c r="E67" s="43" t="s">
         <v>2</v>
       </c>
@@ -2533,11 +2533,11 @@
         <f>A67+1</f>
         <v>57</v>
       </c>
-      <c r="B68" s="60" t="s">
+      <c r="B68" s="66" t="s">
         <v>41</v>
       </c>
-      <c r="C68" s="61"/>
-      <c r="D68" s="62"/>
+      <c r="C68" s="67"/>
+      <c r="D68" s="68"/>
       <c r="E68" s="43" t="s">
         <v>2</v>
       </c>
@@ -2554,11 +2554,11 @@
         <f t="shared" si="0"/>
         <v>58</v>
       </c>
-      <c r="B69" s="60" t="s">
+      <c r="B69" s="66" t="s">
         <v>42</v>
       </c>
-      <c r="C69" s="61"/>
-      <c r="D69" s="62"/>
+      <c r="C69" s="67"/>
+      <c r="D69" s="68"/>
       <c r="E69" s="43" t="s">
         <v>26</v>
       </c>
@@ -2577,11 +2577,11 @@
         <f t="shared" si="0"/>
         <v>59</v>
       </c>
-      <c r="B70" s="60" t="s">
+      <c r="B70" s="66" t="s">
         <v>43</v>
       </c>
-      <c r="C70" s="61"/>
-      <c r="D70" s="62"/>
+      <c r="C70" s="67"/>
+      <c r="D70" s="68"/>
       <c r="E70" s="43" t="s">
         <v>2</v>
       </c>
@@ -2598,9 +2598,9 @@
         <f t="shared" si="0"/>
         <v>60</v>
       </c>
-      <c r="B71" s="79"/>
-      <c r="C71" s="80"/>
-      <c r="D71" s="81"/>
+      <c r="B71" s="84"/>
+      <c r="C71" s="85"/>
+      <c r="D71" s="86"/>
       <c r="E71" s="8"/>
       <c r="F71" s="26"/>
       <c r="G71" s="26"/>
@@ -2611,9 +2611,9 @@
         <f t="shared" si="0"/>
         <v>61</v>
       </c>
-      <c r="B72" s="79"/>
-      <c r="C72" s="80"/>
-      <c r="D72" s="81"/>
+      <c r="B72" s="84"/>
+      <c r="C72" s="85"/>
+      <c r="D72" s="86"/>
       <c r="E72" s="8"/>
       <c r="F72" s="26"/>
       <c r="G72" s="26"/>
@@ -2624,11 +2624,11 @@
         <f t="shared" si="0"/>
         <v>62</v>
       </c>
-      <c r="B73" s="76" t="s">
+      <c r="B73" s="104" t="s">
         <v>24</v>
       </c>
-      <c r="C73" s="77"/>
-      <c r="D73" s="78"/>
+      <c r="C73" s="105"/>
+      <c r="D73" s="106"/>
       <c r="E73" s="58"/>
       <c r="F73" s="25" t="s">
         <v>14</v>
@@ -2645,9 +2645,9 @@
         <f t="shared" si="0"/>
         <v>63</v>
       </c>
-      <c r="B74" s="67"/>
-      <c r="C74" s="68"/>
-      <c r="D74" s="69"/>
+      <c r="B74" s="111"/>
+      <c r="C74" s="112"/>
+      <c r="D74" s="113"/>
       <c r="E74" s="9"/>
       <c r="F74" s="28"/>
       <c r="G74" s="28"/>
@@ -2655,11 +2655,51 @@
     </row>
   </sheetData>
   <mergeCells count="67">
-    <mergeCell ref="B34:D34"/>
-    <mergeCell ref="B35:D35"/>
-    <mergeCell ref="B36:D36"/>
-    <mergeCell ref="B37:D37"/>
-    <mergeCell ref="B32:D32"/>
+    <mergeCell ref="B74:D74"/>
+    <mergeCell ref="B45:D45"/>
+    <mergeCell ref="B46:D46"/>
+    <mergeCell ref="B51:D51"/>
+    <mergeCell ref="B52:D52"/>
+    <mergeCell ref="B62:D62"/>
+    <mergeCell ref="B73:D73"/>
+    <mergeCell ref="B66:D66"/>
+    <mergeCell ref="B63:D63"/>
+    <mergeCell ref="B72:D72"/>
+    <mergeCell ref="B71:D71"/>
+    <mergeCell ref="B69:D69"/>
+    <mergeCell ref="B70:D70"/>
+    <mergeCell ref="B56:D56"/>
+    <mergeCell ref="B44:D44"/>
+    <mergeCell ref="B65:D65"/>
+    <mergeCell ref="H10:H11"/>
+    <mergeCell ref="E10:E11"/>
+    <mergeCell ref="B12:D12"/>
+    <mergeCell ref="B42:D42"/>
+    <mergeCell ref="B39:D39"/>
+    <mergeCell ref="B38:D38"/>
+    <mergeCell ref="B27:D27"/>
+    <mergeCell ref="B68:D68"/>
+    <mergeCell ref="B67:D67"/>
+    <mergeCell ref="B2:D2"/>
+    <mergeCell ref="B10:D10"/>
+    <mergeCell ref="B11:D11"/>
+    <mergeCell ref="B13:D13"/>
+    <mergeCell ref="B9:D9"/>
+    <mergeCell ref="B15:D15"/>
+    <mergeCell ref="B19:D19"/>
+    <mergeCell ref="B14:D14"/>
+    <mergeCell ref="B30:D30"/>
+    <mergeCell ref="B31:D31"/>
+    <mergeCell ref="B16:D16"/>
+    <mergeCell ref="B20:D20"/>
+    <mergeCell ref="B18:D18"/>
+    <mergeCell ref="B17:D17"/>
+    <mergeCell ref="B21:D21"/>
+    <mergeCell ref="B22:D22"/>
+    <mergeCell ref="B23:D23"/>
+    <mergeCell ref="B25:D25"/>
+    <mergeCell ref="B24:D24"/>
+    <mergeCell ref="B26:D26"/>
     <mergeCell ref="B40:D40"/>
     <mergeCell ref="B64:D64"/>
     <mergeCell ref="B60:D60"/>
@@ -2674,54 +2714,14 @@
     <mergeCell ref="B57:D57"/>
     <mergeCell ref="B58:D58"/>
     <mergeCell ref="B59:D59"/>
+    <mergeCell ref="B43:D43"/>
+    <mergeCell ref="B41:D41"/>
+    <mergeCell ref="B34:D34"/>
+    <mergeCell ref="B35:D35"/>
+    <mergeCell ref="B36:D36"/>
+    <mergeCell ref="B37:D37"/>
+    <mergeCell ref="B32:D32"/>
     <mergeCell ref="B33:D33"/>
-    <mergeCell ref="B15:D15"/>
-    <mergeCell ref="B19:D19"/>
-    <mergeCell ref="B14:D14"/>
-    <mergeCell ref="B30:D30"/>
-    <mergeCell ref="B31:D31"/>
-    <mergeCell ref="B2:D2"/>
-    <mergeCell ref="B10:D10"/>
-    <mergeCell ref="B11:D11"/>
-    <mergeCell ref="B13:D13"/>
-    <mergeCell ref="B9:D9"/>
-    <mergeCell ref="B16:D16"/>
-    <mergeCell ref="B43:D43"/>
-    <mergeCell ref="B20:D20"/>
-    <mergeCell ref="B18:D18"/>
-    <mergeCell ref="B17:D17"/>
-    <mergeCell ref="B21:D21"/>
-    <mergeCell ref="B22:D22"/>
-    <mergeCell ref="B23:D23"/>
-    <mergeCell ref="B25:D25"/>
-    <mergeCell ref="B41:D41"/>
-    <mergeCell ref="B24:D24"/>
-    <mergeCell ref="B26:D26"/>
-    <mergeCell ref="B42:D42"/>
-    <mergeCell ref="B39:D39"/>
-    <mergeCell ref="B38:D38"/>
-    <mergeCell ref="B27:D27"/>
-    <mergeCell ref="B68:D68"/>
-    <mergeCell ref="B67:D67"/>
-    <mergeCell ref="B70:D70"/>
-    <mergeCell ref="B56:D56"/>
-    <mergeCell ref="B44:D44"/>
-    <mergeCell ref="B65:D65"/>
-    <mergeCell ref="H10:H11"/>
-    <mergeCell ref="E10:E11"/>
-    <mergeCell ref="B12:D12"/>
-    <mergeCell ref="B74:D74"/>
-    <mergeCell ref="B45:D45"/>
-    <mergeCell ref="B46:D46"/>
-    <mergeCell ref="B51:D51"/>
-    <mergeCell ref="B52:D52"/>
-    <mergeCell ref="B62:D62"/>
-    <mergeCell ref="B73:D73"/>
-    <mergeCell ref="B66:D66"/>
-    <mergeCell ref="B63:D63"/>
-    <mergeCell ref="B72:D72"/>
-    <mergeCell ref="B71:D71"/>
-    <mergeCell ref="B69:D69"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="720" verticalDpi="720" r:id="rId1"/>

</xml_diff>